<commit_message>
Testes DFS e BFS Consertados
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas_Unitario/DFS/PLN_42_10.xlsx
+++ b/Algoritmo_Rota/Planilhas_Unitario/DFS/PLN_42_10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Índice</t>
+          <t>Qtd_Nós</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>Ativos</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -439,138 +439,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ativos</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>melhor rota</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>caminho</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
           <t>Tempo</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Tempo Heuristica</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Tempo Total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>3144</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>34, 10, 1, 23, 4, 13, 40, 25, 35, 33</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12 -&gt; 23 -&gt; 40 -&gt; 35 -&gt; 13 -&gt; 10 -&gt; 4 -&gt; 1 -&gt; 25 -&gt; 33 -&gt; 34 -&gt; 12</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12 -&gt; 16 -&gt; 17 -&gt; 20 -&gt; 24 -&gt; 23 -&gt; 24 -&gt; 32 -&gt; 41 -&gt; 42 -&gt; 40 -&gt; 39 -&gt; 36 -&gt; 35 -&gt; 29 -&gt; 13 -&gt; 12 -&gt; 11 -&gt; 10 -&gt; 7 -&gt; 4 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 25 -&gt; 26 -&gt; 33 -&gt; 27 -&gt; 28 -&gt; 34 -&gt; 28 -&gt; 29 -&gt; 13 -&gt; 12</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>265.1328809261322</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>265.1328809261322</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>24</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2345</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>8, 2, 21, 27, 12, 19, 31, 39, 38, 14</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>24 -&gt; 21 -&gt; 14 -&gt; 12 -&gt; 8 -&gt; 2 -&gt; 27 -&gt; 38 -&gt; 39 -&gt; 31 -&gt; 19 -&gt; 24</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>24 -&gt; 23 -&gt; 22 -&gt; 21 -&gt; 18 -&gt; 14 -&gt; 10 -&gt; 11 -&gt; 12 -&gt; 8 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 25 -&gt; 26 -&gt; 27 -&gt; 28 -&gt; 29 -&gt; 30 -&gt; 37 -&gt; 38 -&gt; 39 -&gt; 38 -&gt; 31 -&gt; 20 -&gt; 19 -&gt; 20 -&gt; 24</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>151.3054983615875</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>151.3054983615875</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2357</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>32, 42, 20, 17, 16, 1, 15, 11, 37, 9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6 -&gt; 9 -&gt; 17 -&gt; 16 -&gt; 20 -&gt; 32 -&gt; 42 -&gt; 37 -&gt; 15 -&gt; 11 -&gt; 1 -&gt; 6</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>6 -&gt; 9 -&gt; 13 -&gt; 17 -&gt; 16 -&gt; 17 -&gt; 20 -&gt; 24 -&gt; 32 -&gt; 41 -&gt; 42 -&gt; 40 -&gt; 39 -&gt; 38 -&gt; 37 -&gt; 30 -&gt; 17 -&gt; 16 -&gt; 15 -&gt; 11 -&gt; 10 -&gt; 7 -&gt; 4 -&gt; 1 -&gt; 2 -&gt; 5 -&gt; 6</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>183.4407358169556</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>183.4407358169556</v>
+      <c r="D2" t="n">
+        <v>441.2654347419739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>